<commit_message>
Updates DB to handle deleting menu objects (categories, items, and mods)
Also updates Menu Editor documentation to remove "varSet" criteria on right side of sheets
</commit_message>
<xml_diff>
--- a/Documentation/MenuEditor.xlsx
+++ b/Documentation/MenuEditor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\CentRes\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7320C35-99FF-4D88-ABF6-8D305A35C39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7DB413-0FAB-4AF4-9323-8EBF86DCF0C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F77EC960-9BAA-439A-A603-3EBA92C13F50}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F77EC960-9BAA-439A-A603-3EBA92C13F50}"/>
   </bookViews>
   <sheets>
     <sheet name="MenuItemEditor.php" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>Menu Title</t>
   </si>
@@ -102,15 +102,6 @@
     <t>Route</t>
   </si>
   <si>
-    <t>The menu editor will be listening for this var to</t>
-  </si>
-  <si>
-    <t>know when to refresh the menu</t>
-  </si>
-  <si>
-    <t>Make sure varSet("updated","true") after you successfully submit</t>
-  </si>
-  <si>
     <t>Category Title</t>
   </si>
   <si>
@@ -121,9 +112,6 @@
   </si>
   <si>
     <t>Parent of "none" has a quickcode of "root"</t>
-  </si>
-  <si>
-    <t>(top of php where you're processing the commit after submitting to self)</t>
   </si>
   <si>
     <t>Menu Category Updated</t>
@@ -235,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +245,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -382,14 +364,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -398,26 +376,29 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -428,28 +409,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,288 +1058,281 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G10"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="2.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.26953125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="3.26953125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:20" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="11" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="1:20" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:20" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="11"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:20" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="11"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:20" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="14"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="13" spans="1:20" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:20" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8" t="s">
+      <c r="C16" s="5"/>
+      <c r="D16" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="12" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P16" s="13" t="s">
+      <c r="P16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R16" s="13" t="s">
+      <c r="R16" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T16" s="13" t="s">
+      <c r="T16" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="R18" s="13" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="R18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T18" s="13" t="s">
+      <c r="T18" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:20" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:20" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="14"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1386,240 +1350,267 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F9B5FB-6061-4B3C-B8EF-104F48F95D82}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08984375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="2.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.26953125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="47.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="15" width="8.7265625" style="5"/>
-    <col min="16" max="20" width="0" style="5" hidden="1" customWidth="1"/>
-    <col min="21" max="16384" width="8.7265625" style="5"/>
+    <col min="1" max="1" width="3.26953125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="2.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.26953125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="47.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="8.7265625" style="3"/>
+    <col min="16" max="20" width="0" style="3" hidden="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:21" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+    </row>
+    <row r="8" spans="1:21" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="4" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="7"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="J9" s="24"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+    </row>
+    <row r="10" spans="1:21" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+    </row>
+    <row r="12" spans="1:21" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:21" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:20" ht="26" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="14"/>
-    </row>
-    <row r="5" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:14" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="14"/>
-      <c r="J7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-    </row>
-    <row r="8" spans="1:14" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="14"/>
-      <c r="J8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="J9" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-    </row>
-    <row r="10" spans="1:14" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="J10" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:14" ht="4.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:20" ht="26" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="14"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="P19" s="13" t="s">
+      <c r="P19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R19" s="13" t="s">
+      <c r="R19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T19" s="13" t="s">
+      <c r="T19" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="R21" s="13" t="s">
+      <c r="R21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="T21" s="13" t="s">
+      <c r="T21" s="8" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1640,7 +1631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACECFAE2-A1C9-4CFB-99D1-71AA59205924}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -1654,148 +1645,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1"/>
+      <c r="B5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-    </row>
-    <row r="2" spans="1:7" ht="8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="1:7" ht="10" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="23"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="26" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="2"/>
-      <c r="B9" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="2"/>
-      <c r="B10" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>